<commit_message>
Added Icon and UI change. Fix the decimal on the export and correct time calculations.
git-svn-id: https://subversion.assembla.com/svn/crm-2013-enterprise-upgrade/trunk/TaskPlayer2@2844 9f9238a3-a6ea-41cf-ad09-a3c91983eb18
</commit_message>
<xml_diff>
--- a/TaskPlayer2/Templates/Report.xlsx
+++ b/TaskPlayer2/Templates/Report.xlsx
@@ -385,18 +385,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -680,7 +679,7 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,20 +695,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B3" t="s">
@@ -735,102 +734,102 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="7" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="6">
         <f>SUBTOTAL(9,B5)</f>
         <v>0</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="6">
         <f t="shared" ref="C6:I6" si="0">SUBTOTAL(9,C5)</f>
         <v>0</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B9" t="s">
@@ -859,102 +858,102 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="7" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="6">
         <f>SUBTOTAL(9,B11)</f>
         <v>0</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="6">
         <f>SUBTOTAL(9,C11)</f>
         <v>0</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="6">
         <f t="shared" ref="D12:I12" si="1">SUBTOTAL(9,D11)</f>
         <v>0</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B15" t="s">
@@ -983,102 +982,102 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="I16" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="I17" s="7" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="6">
         <f>SUBTOTAL(9,B17)</f>
         <v>0</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="6">
         <f>SUBTOTAL(9,C17)</f>
         <v>0</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="6">
         <f t="shared" ref="D18:I18" si="2">SUBTOTAL(9,D17)</f>
         <v>0</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B20" t="s">
@@ -1107,102 +1106,102 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G21" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="H21" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I21" s="3" t="s">
+      <c r="I21" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="I22" s="7" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="6">
         <f>SUBTOTAL(9,B22)</f>
         <v>0</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="6">
         <f>SUBTOTAL(9,C22)</f>
         <v>0</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="6">
         <f t="shared" ref="D23:I23" si="3">SUBTOTAL(9,D22)</f>
         <v>0</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B26" t="s">
@@ -1231,96 +1230,96 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E27" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F27" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="G27" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H27" s="3" t="s">
+      <c r="H27" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I27" s="3" t="s">
+      <c r="I27" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G28" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H28" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="I28" s="1" t="s">
+      <c r="I28" s="7" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="6">
         <f>SUBTOTAL(9,B28)</f>
         <v>0</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="6">
         <f>SUBTOTAL(9,C28)</f>
         <v>0</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="6">
         <f t="shared" ref="D29:I29" si="4">SUBTOTAL(9,D28)</f>
         <v>0</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="6">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="6">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="6">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="6">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I29">
+      <c r="I29" s="6">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>

</xml_diff>